<commit_message>
add app_incidences to Call incidences
</commit_message>
<xml_diff>
--- a/lab_0514.xlsx
+++ b/lab_0514.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="460" windowWidth="28800" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="实验1" sheetId="1" r:id="rId1"/>
     <sheet name="实验2" sheetId="2" r:id="rId2"/>
+    <sheet name="工作表1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="33">
   <si>
     <t>准确率
 (accuracy)</t>
@@ -241,6 +242,35 @@
     <t>units=[n_time_steps*2,n_time_steps]
 dropout=0.4
 activation=relu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n = 12
+n_d = 5
+n_w = 5
+只有事故特征
+正样本比例= 5%，设置了class_weight=1:19</t>
+    <rPh sb="23" eb="24">
+      <t>zhi'you</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>you</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>shi'gu</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>te'z</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>zheng'yang'b</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>bi'li</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>she'zhi'l</t>
+    </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -340,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -380,6 +410,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -660,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView zoomScale="135" workbookViewId="0">
+      <selection activeCell="B7" sqref="A1:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -1115,7 +1151,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="47" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1133,7 +1169,7 @@
       <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8" ht="47" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="10"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1147,7 +1183,7 @@
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A4" s="10"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1161,7 +1197,7 @@
       <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:8" ht="65" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="10"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="7" t="s">
         <v>29</v>
       </c>
@@ -1177,7 +1213,7 @@
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.15">
-      <c r="A6" s="10"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="7" t="s">
         <v>30</v>
       </c>
@@ -1191,7 +1227,7 @@
       <c r="H6" s="9"/>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.15">
-      <c r="A7" s="10"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
@@ -1215,7 +1251,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A8" s="10"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
@@ -1243,4 +1279,212 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.15">
+      <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A2" s="15"/>
+      <c r="B2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="8">
+        <v>0.84460000000000002</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+    </row>
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.15">
+      <c r="A3" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0.84460000000000002</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.15">
+      <c r="A4" s="12"/>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.15">
+      <c r="A5" s="12"/>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" s="12"/>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.15">
+      <c r="A7" s="12"/>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A8" s="12"/>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.15">
+      <c r="A9" s="12"/>
+      <c r="B9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.15">
+      <c r="A10" s="12"/>
+      <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.15">
+      <c r="A11" s="12"/>
+      <c r="B11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A12" s="13"/>
+      <c r="B12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:A12"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>